<commit_message>
improve 1d inversion checking
</commit_message>
<xml_diff>
--- a/inputs/odias_params_new.xlsx
+++ b/inputs/odias_params_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB84C0D-DF40-4145-A674-DEE1749E59A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D52DC-0F4E-459D-967F-AA507D4667FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="3" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
         <v>19</v>
       </c>
       <c r="M9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding higher order Tikhonov - Major
</commit_message>
<xml_diff>
--- a/inputs/odias_params_new.xlsx
+++ b/inputs/odias_params_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D700137-D97C-41F7-959F-386DF02A077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6C82B9-02B4-4DBC-B47E-0DD5462D075B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="62">
   <si>
     <t>fname</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>#1F509A</t>
+  </si>
+  <si>
+    <t>lambda_tk2</t>
+  </si>
+  <si>
+    <t>lambda_tk22</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20AA5E3-18D8-4B5E-AC08-AB63587E2B83}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,15 +561,15 @@
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" customWidth="1"/>
     <col min="7" max="7" width="26" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,25 +595,31 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -632,26 +644,32 @@
       <c r="H2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I2" s="1">
-        <v>15</v>
+      <c r="I2" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2">
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
         <v>23</v>
@@ -659,26 +677,32 @@
       <c r="H3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I3" s="1">
-        <v>15</v>
+      <c r="I3" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K3" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3">
+      <c r="N3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3">
         <v>23</v>
       </c>
-      <c r="N3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
         <v>23</v>
@@ -686,26 +710,32 @@
       <c r="H4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I4" s="1">
-        <v>15</v>
+      <c r="I4" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K4" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>15</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4">
+      <c r="N4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4">
         <v>23</v>
       </c>
-      <c r="N4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
         <v>23</v>
@@ -713,26 +743,32 @@
       <c r="H5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I5" s="1">
-        <v>15</v>
+      <c r="I5" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K5" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5">
+      <c r="N5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5">
         <v>23</v>
       </c>
-      <c r="N5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
         <v>23</v>
@@ -740,26 +776,32 @@
       <c r="H6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I6" s="1">
-        <v>15</v>
+      <c r="I6" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K6" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6">
+      <c r="N6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6">
         <v>23</v>
       </c>
-      <c r="N6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
         <v>23</v>
@@ -767,26 +809,32 @@
       <c r="H7" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I7" s="1">
-        <v>15</v>
+      <c r="I7" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K7" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7">
+      <c r="N7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7">
         <v>23</v>
       </c>
-      <c r="N7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
         <v>23</v>
@@ -794,26 +842,32 @@
       <c r="H8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I8" s="1">
-        <v>15</v>
+      <c r="I8" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K8" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8">
+      <c r="N8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8">
         <v>23</v>
       </c>
-      <c r="N8" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
         <v>22</v>
@@ -821,26 +875,32 @@
       <c r="H9" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I9" s="1">
-        <v>15</v>
+      <c r="I9" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J9" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K9" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>15</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M9">
-        <v>19</v>
-      </c>
-      <c r="N9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>19</v>
+      </c>
+      <c r="P9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
         <v>22</v>
@@ -848,52 +908,72 @@
       <c r="H10" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I10" s="1">
-        <v>15</v>
+      <c r="I10" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J10" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K10" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M10">
-        <v>19</v>
-      </c>
-      <c r="N10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>19</v>
+      </c>
+      <c r="P10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -902,10 +982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069A6CBD-9180-4207-8C39-A2C64C8EF28F}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,13 +997,13 @@
     <col min="5" max="5" width="25.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,25 +1029,31 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -992,26 +1078,32 @@
       <c r="H2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I2" s="1">
-        <v>15</v>
+      <c r="I2" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="G3" s="5" t="s">
         <v>38</v>
@@ -1019,26 +1111,32 @@
       <c r="H3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I3" s="1">
-        <v>15</v>
+      <c r="I3" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K3" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3">
-        <v>19</v>
-      </c>
-      <c r="N3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>19</v>
+      </c>
+      <c r="P3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="G4" s="5" t="s">
         <v>39</v>
@@ -1046,26 +1144,32 @@
       <c r="H4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I4" s="1">
-        <v>15</v>
+      <c r="I4" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K4" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>15</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4">
-        <v>19</v>
-      </c>
-      <c r="N4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4">
+        <v>19</v>
+      </c>
+      <c r="P4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
       <c r="G5" s="5" t="s">
         <v>39</v>
@@ -1073,26 +1177,32 @@
       <c r="H5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I5" s="1">
-        <v>15</v>
+      <c r="I5" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K5" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M5">
-        <v>19</v>
-      </c>
-      <c r="N5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>19</v>
+      </c>
+      <c r="P5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
       <c r="G6" s="5" t="s">
         <v>40</v>
@@ -1100,26 +1210,32 @@
       <c r="H6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I6" s="1">
-        <v>15</v>
+      <c r="I6" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K6" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6">
-        <v>19</v>
-      </c>
-      <c r="N6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6">
+        <v>19</v>
+      </c>
+      <c r="P6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
         <v>41</v>
@@ -1127,26 +1243,32 @@
       <c r="H7" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I7" s="1">
-        <v>15</v>
+      <c r="I7" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K7" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M7">
-        <v>19</v>
-      </c>
-      <c r="N7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>19</v>
+      </c>
+      <c r="P7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="G8" s="5" t="s">
         <v>42</v>
@@ -1154,26 +1276,32 @@
       <c r="H8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I8" s="1">
-        <v>15</v>
+      <c r="I8" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K8" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8">
-        <v>19</v>
-      </c>
-      <c r="N8" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8">
+        <v>19</v>
+      </c>
+      <c r="P8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="G9" s="5" t="s">
         <v>43</v>
@@ -1181,26 +1309,32 @@
       <c r="H9" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I9" s="1">
-        <v>15</v>
+      <c r="I9" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J9" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K9" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>15</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M9">
-        <v>19</v>
-      </c>
-      <c r="N9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>19</v>
+      </c>
+      <c r="P9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
       <c r="G10" s="5" t="s">
         <v>44</v>
@@ -1208,26 +1342,32 @@
       <c r="H10" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I10" s="1">
-        <v>15</v>
+      <c r="I10" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J10" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K10" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10">
-        <v>19</v>
-      </c>
-      <c r="N10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10">
+        <v>19</v>
+      </c>
+      <c r="P10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
       <c r="G11" s="5" t="s">
         <v>45</v>
@@ -1235,26 +1375,32 @@
       <c r="H11" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I11" s="1">
-        <v>15</v>
+      <c r="I11" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J11" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K11" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K11" s="1">
+        <v>15</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M11">
-        <v>19</v>
-      </c>
-      <c r="N11" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>19</v>
+      </c>
+      <c r="P11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
       <c r="G12" s="5" t="s">
         <v>46</v>
@@ -1262,26 +1408,32 @@
       <c r="H12" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I12" s="1">
-        <v>15</v>
+      <c r="I12" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K12" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>15</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12">
-        <v>19</v>
-      </c>
-      <c r="N12" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12">
+        <v>19</v>
+      </c>
+      <c r="P12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
       <c r="G13" s="5" t="s">
         <v>47</v>
@@ -1289,26 +1441,32 @@
       <c r="H13" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I13" s="1">
-        <v>15</v>
+      <c r="I13" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J13" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>15</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M13">
-        <v>19</v>
-      </c>
-      <c r="N13" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>19</v>
+      </c>
+      <c r="P13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E14" s="2"/>
       <c r="G14" s="5" t="s">
         <v>48</v>
@@ -1316,26 +1474,32 @@
       <c r="H14" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I14" s="1">
-        <v>15</v>
+      <c r="I14" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J14" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K14" s="1">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14">
-        <v>19</v>
-      </c>
-      <c r="N14" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14">
+        <v>19</v>
+      </c>
+      <c r="P14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
       <c r="G15" s="5" t="s">
         <v>49</v>
@@ -1343,26 +1507,32 @@
       <c r="H15" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I15" s="1">
-        <v>15</v>
+      <c r="I15" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J15" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>15</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M15">
-        <v>19</v>
-      </c>
-      <c r="N15" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>19</v>
+      </c>
+      <c r="P15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
       <c r="G16" s="5" t="s">
         <v>50</v>
@@ -1370,26 +1540,32 @@
       <c r="H16" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I16" s="1">
-        <v>15</v>
+      <c r="I16" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J16" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K16" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K16" s="1">
+        <v>15</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16">
-        <v>19</v>
-      </c>
-      <c r="N16" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16">
+        <v>19</v>
+      </c>
+      <c r="P16" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E17" s="2"/>
       <c r="G17" s="5" t="s">
         <v>51</v>
@@ -1397,22 +1573,28 @@
       <c r="H17" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I17" s="1">
-        <v>15</v>
+      <c r="I17" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J17" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K17" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K17" s="1">
+        <v>15</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M17">
-        <v>19</v>
-      </c>
-      <c r="N17" s="1" t="b">
+      <c r="O17">
+        <v>19</v>
+      </c>
+      <c r="P17" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1423,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5E4505-E9C8-42A1-8718-1B515BF5CEF0}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,14 +1620,14 @@
     <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="10" width="13.5703125" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1471,25 +1653,31 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1514,26 +1702,32 @@
       <c r="H2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I2" s="1">
-        <v>15</v>
+      <c r="I2" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="G3" s="5" t="s">
         <v>53</v>
@@ -1541,26 +1735,32 @@
       <c r="H3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I3" s="1">
-        <v>15</v>
+      <c r="I3" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K3" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="1">
-        <v>19</v>
-      </c>
-      <c r="N3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="1">
+        <v>19</v>
+      </c>
+      <c r="P3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="G4" s="5" t="s">
         <v>54</v>
@@ -1568,26 +1768,32 @@
       <c r="H4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I4" s="1">
-        <v>15</v>
+      <c r="I4" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K4" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>15</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="1">
-        <v>19</v>
-      </c>
-      <c r="N4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="1">
+        <v>19</v>
+      </c>
+      <c r="P4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
       <c r="G5" s="5" t="s">
         <v>55</v>
@@ -1595,26 +1801,32 @@
       <c r="H5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I5" s="1">
-        <v>15</v>
+      <c r="I5" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K5" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="1">
-        <v>19</v>
-      </c>
-      <c r="N5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="1">
+        <v>19</v>
+      </c>
+      <c r="P5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
       <c r="G6" s="5" t="s">
         <v>56</v>
@@ -1622,26 +1834,32 @@
       <c r="H6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I6" s="1">
-        <v>15</v>
+      <c r="I6" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K6" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="1">
-        <v>19</v>
-      </c>
-      <c r="N6" s="1" t="b">
+      <c r="N6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="1">
+        <v>19</v>
+      </c>
+      <c r="P6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
         <v>57</v>
@@ -1649,26 +1867,32 @@
       <c r="H7" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I7" s="1">
-        <v>15</v>
+      <c r="I7" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K7" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="1">
-        <v>19</v>
-      </c>
-      <c r="N7" s="1" t="b">
+      <c r="N7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="1">
+        <v>19</v>
+      </c>
+      <c r="P7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="G8" s="5" t="s">
         <v>58</v>
@@ -1676,28 +1900,34 @@
       <c r="H8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="I8" s="1">
-        <v>15</v>
+      <c r="I8" s="2">
+        <v>1E-4</v>
       </c>
       <c r="J8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K8" s="1" t="s">
+        <v>1E-4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="1">
-        <v>19</v>
-      </c>
-      <c r="N8" s="1" t="b">
+      <c r="N8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="1">
+        <v>19</v>
+      </c>
+      <c r="P8" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
-      <c r="L9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Averaging distributions added - exponential distance added
</commit_message>
<xml_diff>
--- a/inputs/odias_params_new.xlsx
+++ b/inputs/odias_params_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8192DB9E-3192-4554-8F3A-9C5B4A006110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378BA74E-00AF-43E8-9957-1BA8A5D1344A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ET017_NIT013_AIR16_DIST" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="94">
   <si>
     <t>fname</t>
   </si>
@@ -224,9 +224,6 @@
     <t>lambda_tk2</t>
   </si>
   <si>
-    <t>lambda_tk22</t>
-  </si>
-  <si>
     <t>2024-07-26_143650_SMPS</t>
   </si>
   <si>
@@ -318,6 +315,12 @@
   </si>
   <si>
     <t>ET017_NIT013_AIR16_DIST</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>lambda_ed</t>
   </si>
 </sst>
 </file>
@@ -657,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE5B189-3795-4D9F-8470-DCFD19DE4918}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:P17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +681,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +710,7 @@
         <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -727,13 +730,16 @@
       <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -754,10 +760,10 @@
         <v>1E-4</v>
       </c>
       <c r="I2" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K2" s="1">
         <v>15</v>
@@ -766,72 +772,78 @@
         <v>1000</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2">
-        <v>19</v>
-      </c>
-      <c r="P2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="5" t="s">
+      <c r="N3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3">
+        <v>19</v>
+      </c>
+      <c r="P3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K3" s="1">
-        <v>15</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="H4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>15</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3">
-        <v>19</v>
-      </c>
-      <c r="P3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K4" s="1">
-        <v>15</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="N4" s="6" t="s">
         <v>19</v>
       </c>
@@ -841,125 +853,137 @@
       <c r="P4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5">
+        <v>19</v>
+      </c>
+      <c r="P5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K5" s="1">
-        <v>15</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="H6" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5">
-        <v>19</v>
-      </c>
-      <c r="P5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G6" s="5" t="s">
+      <c r="N6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6">
+        <v>19</v>
+      </c>
+      <c r="P6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K6" s="1">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="H7" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6">
-        <v>19</v>
-      </c>
-      <c r="P6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G7" s="5" t="s">
+      <c r="N7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7">
+        <v>19</v>
+      </c>
+      <c r="P7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K7" s="1">
-        <v>15</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="H8" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7">
-        <v>19</v>
-      </c>
-      <c r="P7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G8" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>15</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="N8" s="6" t="s">
         <v>19</v>
       </c>
@@ -969,14 +993,13 @@
       <c r="P8" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
         <v>47</v>
       </c>
@@ -984,10 +1007,10 @@
         <v>1E-4</v>
       </c>
       <c r="I9" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K9" s="1">
         <v>15</v>
@@ -996,72 +1019,78 @@
         <v>1000</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9">
+        <v>19</v>
+      </c>
+      <c r="P9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K10" s="1">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9">
-        <v>19</v>
-      </c>
-      <c r="P9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G10" s="5" t="s">
+      <c r="N10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10">
+        <v>19</v>
+      </c>
+      <c r="P10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K10" s="1">
-        <v>15</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="H11" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>15</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10">
-        <v>19</v>
-      </c>
-      <c r="P10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K11" s="1">
-        <v>15</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="N11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1071,125 +1100,137 @@
       <c r="P11" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>15</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12">
+        <v>19</v>
+      </c>
+      <c r="P12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K12" s="1">
-        <v>15</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="H13" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>15</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12">
-        <v>19</v>
-      </c>
-      <c r="P12" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
+      <c r="N13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13">
+        <v>19</v>
+      </c>
+      <c r="P13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K13" s="1">
-        <v>15</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="H14" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13">
-        <v>19</v>
-      </c>
-      <c r="P13" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
+      <c r="N14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14">
+        <v>19</v>
+      </c>
+      <c r="P14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K14" s="1">
-        <v>15</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="H15" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K15" s="1">
+        <v>15</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14">
-        <v>19</v>
-      </c>
-      <c r="P14" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K15" s="1">
-        <v>15</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="N15" s="6" t="s">
         <v>19</v>
       </c>
@@ -1199,8 +1240,11 @@
       <c r="P15" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>25</v>
       </c>
@@ -1208,58 +1252,61 @@
         <v>26</v>
       </c>
       <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K16" s="1">
+        <v>15</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16">
+        <v>19</v>
+      </c>
+      <c r="P16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K16" s="1">
-        <v>15</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="H17" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>15</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16">
-        <v>19</v>
-      </c>
-      <c r="P16" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="K17" s="1">
-        <v>15</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="N17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1269,20 +1316,23 @@
       <c r="P17" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1298,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069A6CBD-9180-4207-8C39-A2C64C8EF28F}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1396,7 @@
         <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1393,10 +1443,10 @@
         <v>1E-4</v>
       </c>
       <c r="I2" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K2" s="1">
         <v>15</v>
@@ -1426,10 +1476,10 @@
         <v>1E-4</v>
       </c>
       <c r="I3" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J3" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K3" s="1">
         <v>15</v>
@@ -1459,10 +1509,10 @@
         <v>1E-4</v>
       </c>
       <c r="I4" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K4" s="1">
         <v>15</v>
@@ -1492,10 +1542,10 @@
         <v>1E-4</v>
       </c>
       <c r="I5" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K5" s="1">
         <v>15</v>
@@ -1525,10 +1575,10 @@
         <v>1E-4</v>
       </c>
       <c r="I6" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K6" s="1">
         <v>15</v>
@@ -1558,10 +1608,10 @@
         <v>1E-4</v>
       </c>
       <c r="I7" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J7" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K7" s="1">
         <v>15</v>
@@ -1591,10 +1641,10 @@
         <v>1E-4</v>
       </c>
       <c r="I8" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J8" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K8" s="1">
         <v>15</v>
@@ -1624,10 +1674,10 @@
         <v>1E-4</v>
       </c>
       <c r="I9" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K9" s="1">
         <v>15</v>
@@ -1657,10 +1707,10 @@
         <v>1E-4</v>
       </c>
       <c r="I10" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J10" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K10" s="1">
         <v>15</v>
@@ -1690,10 +1740,10 @@
         <v>1E-4</v>
       </c>
       <c r="I11" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J11" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K11" s="1">
         <v>15</v>
@@ -1723,10 +1773,10 @@
         <v>1E-4</v>
       </c>
       <c r="I12" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J12" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K12" s="1">
         <v>15</v>
@@ -1756,10 +1806,10 @@
         <v>1E-4</v>
       </c>
       <c r="I13" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J13" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K13" s="1">
         <v>15</v>
@@ -1789,10 +1839,10 @@
         <v>1E-4</v>
       </c>
       <c r="I14" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J14" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K14" s="1">
         <v>15</v>
@@ -1822,10 +1872,10 @@
         <v>1E-4</v>
       </c>
       <c r="I15" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J15" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K15" s="1">
         <v>15</v>
@@ -1855,10 +1905,10 @@
         <v>1E-4</v>
       </c>
       <c r="I16" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J16" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K16" s="1">
         <v>15</v>
@@ -1888,10 +1938,10 @@
         <v>1E-4</v>
       </c>
       <c r="I17" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J17" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K17" s="1">
         <v>15</v>
@@ -1922,7 +1972,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +2020,7 @@
         <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -2017,10 +2067,10 @@
         <v>1E-4</v>
       </c>
       <c r="I2" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K2" s="1">
         <v>15</v>
@@ -2050,10 +2100,10 @@
         <v>1E-4</v>
       </c>
       <c r="I3" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J3" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K3" s="1">
         <v>15</v>
@@ -2083,10 +2133,10 @@
         <v>1E-4</v>
       </c>
       <c r="I4" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K4" s="1">
         <v>15</v>
@@ -2116,10 +2166,10 @@
         <v>1E-4</v>
       </c>
       <c r="I5" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K5" s="1">
         <v>15</v>
@@ -2149,10 +2199,10 @@
         <v>1E-4</v>
       </c>
       <c r="I6" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K6" s="1">
         <v>15</v>
@@ -2182,10 +2232,10 @@
         <v>1E-4</v>
       </c>
       <c r="I7" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J7" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K7" s="1">
         <v>15</v>
@@ -2215,10 +2265,10 @@
         <v>1E-4</v>
       </c>
       <c r="I8" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J8" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K8" s="1">
         <v>15</v>
@@ -2253,7 +2303,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,7 +2352,7 @@
         <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -2349,10 +2399,10 @@
         <v>1E-4</v>
       </c>
       <c r="I2" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K2" s="1">
         <v>15</v>
@@ -2382,10 +2432,10 @@
         <v>1E-4</v>
       </c>
       <c r="I3" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J3" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K3" s="1">
         <v>15</v>
@@ -2415,10 +2465,10 @@
         <v>1E-4</v>
       </c>
       <c r="I4" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K4" s="1">
         <v>15</v>
@@ -2448,10 +2498,10 @@
         <v>1E-4</v>
       </c>
       <c r="I5" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K5" s="1">
         <v>15</v>
@@ -2481,10 +2531,10 @@
         <v>1E-4</v>
       </c>
       <c r="I6" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K6" s="1">
         <v>15</v>
@@ -2514,10 +2564,10 @@
         <v>1E-4</v>
       </c>
       <c r="I7" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J7" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K7" s="1">
         <v>15</v>
@@ -2547,10 +2597,10 @@
         <v>1E-4</v>
       </c>
       <c r="I8" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J8" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K8" s="1">
         <v>15</v>
@@ -2580,10 +2630,10 @@
         <v>1E-4</v>
       </c>
       <c r="I9" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K9" s="1">
         <v>15</v>
@@ -2613,10 +2663,10 @@
         <v>1E-4</v>
       </c>
       <c r="I10" s="2">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J10" s="2">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K10" s="1">
         <v>15</v>

</xml_diff>